<commit_message>
update app for IN variant input
</commit_message>
<xml_diff>
--- a/Inputs/CAcounties.xlsx
+++ b/Inputs/CAcounties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A939F0D-A164-634A-90D3-72318EDE29C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4509B38B-D3BF-394D-B7AD-2A40A2817C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30740" windowHeight="15040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30740" windowHeight="15040" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="162">
   <si>
     <t>Number of Days from Infection to Becoming Infectious (Latent Period)</t>
   </si>
@@ -517,6 +517,9 @@
   </si>
   <si>
     <t>duration_natural_years</t>
+  </si>
+  <si>
+    <t>IN</t>
   </si>
 </sst>
 </file>
@@ -629,7 +632,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -702,12 +705,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -843,22 +857,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -869,6 +883,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1770,53 +1786,53 @@
   <sheetData>
     <row r="1" spans="1:13" s="33" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="32"/>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="75" t="s">
+      <c r="C1" s="76"/>
+      <c r="D1" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75" t="s">
+      <c r="E1" s="77"/>
+      <c r="F1" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="75"/>
-      <c r="H1" s="78" t="s">
+      <c r="G1" s="77"/>
+      <c r="H1" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="78"/>
-      <c r="J1" s="75" t="s">
+      <c r="I1" s="76"/>
+      <c r="J1" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75" t="s">
+      <c r="K1" s="77"/>
+      <c r="L1" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="75"/>
+      <c r="M1" s="77"/>
     </row>
     <row r="2" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34"/>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="76" t="s">
+      <c r="E2" s="75"/>
+      <c r="F2" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="79" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="75" t="s">
         <v>117</v>
       </c>
-      <c r="I2" s="79"/>
-      <c r="J2" s="76" t="s">
+      <c r="I2" s="75"/>
+      <c r="J2" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="77"/>
+      <c r="K2" s="79"/>
       <c r="L2" s="35" t="s">
         <v>119</v>
       </c>
@@ -2027,17 +2043,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A43:A487 A5:A36" xr:uid="{DFFBA6CA-6EEC-F54F-9268-B981437AD2EB}">
@@ -2058,7 +2074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E08ED19-209C-1244-95CD-D0E05E30CCAF}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2662,8 +2678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1D40A3-9166-4938-BDA5-A18F4C1841F8}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3059,6 +3075,56 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="83" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="11">
+        <v>44221</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="83">
+        <v>2.25</v>
+      </c>
+      <c r="E9" s="83">
+        <v>1</v>
+      </c>
+      <c r="F9" s="83">
+        <v>1</v>
+      </c>
+      <c r="G9" s="83">
+        <v>1</v>
+      </c>
+      <c r="H9" s="83">
+        <v>1</v>
+      </c>
+      <c r="I9" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="84">
+        <v>0.85</v>
+      </c>
+      <c r="K9" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="M9" s="84">
+        <v>0.85</v>
+      </c>
+      <c r="N9" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="O9" s="83">
+        <v>5</v>
+      </c>
+      <c r="P9" s="83">
+        <v>5</v>
+      </c>
+    </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I10" s="73"/>
       <c r="J10" s="73"/>

</xml_diff>